<commit_message>
Refactorizacion general de aplicacion a version v2.0-alpha
Refactorizacion general de la aplicacion para mejorar
el sistema de comunicacion entre el frontend y el backend,
así como la estructura de archivos y la organización del código.
Sistema en fase alpha.
</commit_message>
<xml_diff>
--- a/bd/ruta.xlsx
+++ b/bd/ruta.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L138"/>
+  <dimension ref="A1:L137"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -613,125 +613,116 @@
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="11">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>20250318</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D3" s="9" t="inlineStr">
         <is>
           <t>9999</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ACHS Osorno</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Av Zenteno 1529</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Osorno</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>DOCTOR SIMI</t>
+        </is>
+      </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>mall valdivia</t>
+        </is>
+      </c>
+      <c r="G3" s="9" t="inlineStr">
+        <is>
+          <t>valdivia</t>
+        </is>
+      </c>
+      <c r="H3" s="9" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="9" t="inlineStr">
+        <is>
+          <t>SERVICIO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="J3" s="9" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="11">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>20250318</t>
-        </is>
-      </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t>9999</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>DOCTOR SIMI</t>
-        </is>
-      </c>
-      <c r="F4" s="9" t="inlineStr">
-        <is>
-          <t>mall valdivia</t>
-        </is>
-      </c>
-      <c r="G4" s="9" t="inlineStr">
-        <is>
-          <t>valdivia</t>
-        </is>
-      </c>
-      <c r="H4" s="9" t="inlineStr">
+      <c r="A4" s="14" t="n">
+        <v>20250318</v>
+      </c>
+      <c r="B4" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15" t="n">
+        <v>9999</v>
+      </c>
+      <c r="E4" s="15" t="inlineStr">
+        <is>
+          <t>ACHS VALDIVIA</t>
+        </is>
+      </c>
+      <c r="F4" s="15" t="inlineStr">
+        <is>
+          <t>Beauchef Nº705, Valdivia</t>
+        </is>
+      </c>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t>Valdivia</t>
+        </is>
+      </c>
+      <c r="H4" s="14" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I4" s="9" t="inlineStr">
-        <is>
-          <t>SERVICIO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="J4" s="9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="I4" s="14" t="n"/>
+      <c r="J4" s="16" t="n"/>
     </row>
     <row r="5" ht="15" customHeight="1" s="11">
       <c r="A5" s="14" t="n">
         <v>20250318</v>
       </c>
       <c r="B5" s="15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>15</v>
-      </c>
-      <c r="D5" s="15" t="n">
-        <v>9999</v>
+        <v>60</v>
+      </c>
+      <c r="D5" s="15" t="inlineStr">
+        <is>
+          <t>77.880.747-5</t>
+        </is>
       </c>
       <c r="E5" s="15" t="inlineStr">
         <is>
-          <t>ACHS VALDIVIA</t>
+          <t>Salud Humana Pablo Contreras</t>
         </is>
       </c>
       <c r="F5" s="15" t="inlineStr">
         <is>
-          <t>Beauchef Nº705, Valdivia</t>
+          <t>beauchef 925  ( nueva direccion)</t>
         </is>
       </c>
       <c r="G5" s="14" t="inlineStr">
@@ -739,12 +730,14 @@
           <t>Valdivia</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr">
+      <c r="H5" s="14" t="n">
+        <v>966796589</v>
+      </c>
+      <c r="I5" s="14" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I5" s="14" t="n"/>
       <c r="J5" s="16" t="n"/>
     </row>
     <row r="6" ht="15" customHeight="1" s="11">
@@ -752,24 +745,24 @@
         <v>20250318</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D6" s="15" t="inlineStr">
         <is>
-          <t>77.880.747-5</t>
+          <t>77.624.403-1</t>
         </is>
       </c>
       <c r="E6" s="15" t="inlineStr">
         <is>
-          <t>Salud Humana Pablo Contreras</t>
+          <t>serv para salud humana Gloria Jofré EIRL</t>
         </is>
       </c>
       <c r="F6" s="15" t="inlineStr">
         <is>
-          <t>beauchef 925  ( nueva direccion)</t>
+          <t>García Reyes 686</t>
         </is>
       </c>
       <c r="G6" s="14" t="inlineStr">
@@ -778,11 +771,11 @@
         </is>
       </c>
       <c r="H6" s="14" t="n">
-        <v>966796589</v>
+        <v>952541245</v>
       </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>DEUDA</t>
         </is>
       </c>
       <c r="J6" s="16" t="n"/>
@@ -792,37 +785,37 @@
         <v>20250318</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D7" s="15" t="inlineStr">
         <is>
-          <t>77.624.403-1</t>
+          <t>65.062.843-8</t>
         </is>
       </c>
       <c r="E7" s="15" t="inlineStr">
         <is>
-          <t>serv para salud humana Gloria Jofré EIRL</t>
+          <t>Fundacion salud y Familia</t>
         </is>
       </c>
       <c r="F7" s="15" t="inlineStr">
         <is>
-          <t>García Reyes 686</t>
+          <t>Benavente 379 of 206</t>
         </is>
       </c>
       <c r="G7" s="14" t="inlineStr">
         <is>
-          <t>Valdivia</t>
+          <t>Puerto Montt</t>
         </is>
       </c>
       <c r="H7" s="14" t="n">
-        <v>952541245</v>
+        <v>987516103</v>
       </c>
       <c r="I7" s="14" t="inlineStr">
         <is>
-          <t>DEUDA</t>
+          <t>a las 16:00 / nesecita 100 bolsas amarillas</t>
         </is>
       </c>
       <c r="J7" s="16" t="n"/>
@@ -832,24 +825,22 @@
         <v>20250318</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="15" t="inlineStr">
-        <is>
-          <t>65.062.843-8</t>
-        </is>
+        <v>15</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>9999</v>
       </c>
       <c r="E8" s="15" t="inlineStr">
         <is>
-          <t>Fundacion salud y Familia</t>
+          <t>ACHS PUERTO MONTT</t>
         </is>
       </c>
       <c r="F8" s="15" t="inlineStr">
         <is>
-          <t>Benavente 379 of 206</t>
+          <t>Ejército Nº360</t>
         </is>
       </c>
       <c r="G8" s="14" t="inlineStr">
@@ -857,14 +848,12 @@
           <t>Puerto Montt</t>
         </is>
       </c>
-      <c r="H8" s="14" t="n">
-        <v>987516103</v>
-      </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>a las 16:00 / nesecita 100 bolsas amarillas</t>
-        </is>
-      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="n"/>
       <c r="J8" s="16" t="n"/>
     </row>
     <row r="9" ht="15" customHeight="1" s="11">
@@ -872,22 +861,22 @@
         <v>20250318</v>
       </c>
       <c r="B9" s="15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="15" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>9999</v>
       </c>
       <c r="E9" s="15" t="inlineStr">
         <is>
-          <t>ACHS PUERTO MONTT</t>
+          <t>EVEREST PTO MONTT</t>
         </is>
       </c>
       <c r="F9" s="15" t="inlineStr">
         <is>
-          <t>Ejército Nº360</t>
+          <t>Juan Soler Manfredini L 131</t>
         </is>
       </c>
       <c r="G9" s="14" t="inlineStr">
@@ -900,7 +889,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I9" s="14" t="n"/>
+      <c r="I9" s="14" t="inlineStr">
+        <is>
+          <t>8:30 a 13 y 14 a 19</t>
+        </is>
+      </c>
       <c r="J9" s="16" t="n"/>
     </row>
     <row r="10" ht="15" customHeight="1" s="11">
@@ -908,22 +901,24 @@
         <v>20250318</v>
       </c>
       <c r="B10" s="15" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="15" t="n">
         <v>30</v>
       </c>
-      <c r="D10" s="15" t="n">
-        <v>9999</v>
+      <c r="D10" s="15" t="inlineStr">
+        <is>
+          <t>65.062.843-8</t>
+        </is>
       </c>
       <c r="E10" s="15" t="inlineStr">
         <is>
-          <t>EVEREST PTO MONTT</t>
+          <t>CESFAM San Pablo</t>
         </is>
       </c>
       <c r="F10" s="15" t="inlineStr">
         <is>
-          <t>Juan Soler Manfredini L 131</t>
+          <t>Barrancas S/N mirasol</t>
         </is>
       </c>
       <c r="G10" s="14" t="inlineStr">
@@ -931,14 +926,12 @@
           <t>Puerto Montt</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="H10" s="14" t="n">
+        <v>990579442</v>
       </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
-          <t>8:30 a 13 y 14 a 19</t>
+          <t>9:30 a 14 y 17:30 a 20</t>
         </is>
       </c>
       <c r="J10" s="16" t="n"/>
@@ -948,24 +941,24 @@
         <v>20250318</v>
       </c>
       <c r="B11" s="15" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="15" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>65.062.843-8</t>
+          <t>77.628.398-3</t>
         </is>
       </c>
       <c r="E11" s="15" t="inlineStr">
         <is>
-          <t>CESFAM San Pablo</t>
+          <t>CLINICA ODONTOLOGICA ACDENT SPA</t>
         </is>
       </c>
       <c r="F11" s="15" t="inlineStr">
         <is>
-          <t>Barrancas S/N mirasol</t>
+          <t>Antonio Varas 55 of 509</t>
         </is>
       </c>
       <c r="G11" s="14" t="inlineStr">
@@ -973,12 +966,14 @@
           <t>Puerto Montt</t>
         </is>
       </c>
-      <c r="H11" s="14" t="n">
-        <v>990579442</v>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>964988313/967120480</t>
+        </is>
       </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
-          <t>9:30 a 14 y 17:30 a 20</t>
+          <t>10 a 13 y 15 a 17:30</t>
         </is>
       </c>
       <c r="J11" s="16" t="n"/>
@@ -988,24 +983,24 @@
         <v>20250318</v>
       </c>
       <c r="B12" s="15" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>77.628.398-3</t>
+          <t>77.491.661-k</t>
         </is>
       </c>
       <c r="E12" s="15" t="inlineStr">
         <is>
-          <t>CLINICA ODONTOLOGICA ACDENT SPA</t>
+          <t>Emuna soluciones medicas spa</t>
         </is>
       </c>
       <c r="F12" s="15" t="inlineStr">
         <is>
-          <t>Antonio Varas 55 of 509</t>
+          <t>Benavente 840,Of 605</t>
         </is>
       </c>
       <c r="G12" s="14" t="inlineStr">
@@ -1015,12 +1010,12 @@
       </c>
       <c r="H12" s="14" t="inlineStr">
         <is>
-          <t>964988313/967120480</t>
+          <t>962826997/951701572</t>
         </is>
       </c>
       <c r="I12" s="14" t="inlineStr">
         <is>
-          <t>10 a 13 y 15 a 17:30</t>
+          <t>9 a 13 y 14 a 16:00</t>
         </is>
       </c>
       <c r="J12" s="16" t="n"/>
@@ -1030,24 +1025,24 @@
         <v>20250318</v>
       </c>
       <c r="B13" s="15" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D13" s="15" t="inlineStr">
         <is>
-          <t>77.491.661-k</t>
+          <t>76.058.615-3</t>
         </is>
       </c>
       <c r="E13" s="15" t="inlineStr">
         <is>
-          <t>Emuna soluciones medicas spa</t>
+          <t>Fernandez y Haussmann odontologia</t>
         </is>
       </c>
       <c r="F13" s="15" t="inlineStr">
         <is>
-          <t>Benavente 840,Of 605</t>
+          <t>Quillota 175 of 1110</t>
         </is>
       </c>
       <c r="G13" s="14" t="inlineStr">
@@ -1057,12 +1052,12 @@
       </c>
       <c r="H13" s="14" t="inlineStr">
         <is>
-          <t>962826997/951701572</t>
+          <t>652263740/934533835</t>
         </is>
       </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
-          <t>9 a 13 y 14 a 16:00</t>
+          <t>10 a 18</t>
         </is>
       </c>
       <c r="J13" s="16" t="n"/>
@@ -1072,24 +1067,24 @@
         <v>20250318</v>
       </c>
       <c r="B14" s="15" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D14" s="15" t="inlineStr">
         <is>
-          <t>76.058.615-3</t>
+          <t>78.034.130-0</t>
         </is>
       </c>
       <c r="E14" s="15" t="inlineStr">
         <is>
-          <t>Fernandez y Haussmann odontologia</t>
+          <t>KARUS</t>
         </is>
       </c>
       <c r="F14" s="15" t="inlineStr">
         <is>
-          <t>Quillota 175 of 1110</t>
+          <t>Juan soler manfredini 41 of 1803</t>
         </is>
       </c>
       <c r="G14" s="14" t="inlineStr">
@@ -1099,12 +1094,12 @@
       </c>
       <c r="H14" s="14" t="inlineStr">
         <is>
-          <t>652263740/934533835</t>
+          <t>952296251/957121954</t>
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr">
         <is>
-          <t>10 a 18</t>
+          <t>cliente nuevo 1C Y 1B /11 a  14</t>
         </is>
       </c>
       <c r="J14" s="16" t="n"/>
@@ -1114,24 +1109,24 @@
         <v>20250318</v>
       </c>
       <c r="B15" s="15" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D15" s="15" t="inlineStr">
         <is>
-          <t>78.034.130-0</t>
+          <t>77.962.205-3</t>
         </is>
       </c>
       <c r="E15" s="15" t="inlineStr">
         <is>
-          <t>KARUS</t>
+          <t>we face and body spa.</t>
         </is>
       </c>
       <c r="F15" s="15" t="inlineStr">
         <is>
-          <t>Juan soler manfredini 41 of 1803</t>
+          <t>O´higgins 167 of 609</t>
         </is>
       </c>
       <c r="G15" s="14" t="inlineStr">
@@ -1139,14 +1134,12 @@
           <t>Puerto Montt</t>
         </is>
       </c>
-      <c r="H15" s="14" t="inlineStr">
-        <is>
-          <t>952296251/957121954</t>
-        </is>
+      <c r="H15" s="14" t="n">
+        <v>972078066</v>
       </c>
       <c r="I15" s="14" t="inlineStr">
         <is>
-          <t>cliente nuevo 1C Y 1B /11 a  14</t>
+          <t>10 a 19</t>
         </is>
       </c>
       <c r="J15" s="16" t="n"/>
@@ -1156,24 +1149,24 @@
         <v>20250318</v>
       </c>
       <c r="B16" s="15" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D16" s="15" t="inlineStr">
         <is>
-          <t>77.962.205-3</t>
+          <t>77.141.688-8</t>
         </is>
       </c>
       <c r="E16" s="15" t="inlineStr">
         <is>
-          <t>we face and body spa.</t>
+          <t>Servicios Sociales Sur Spa</t>
         </is>
       </c>
       <c r="F16" s="15" t="inlineStr">
         <is>
-          <t>O´higgins 167 of 609</t>
+          <t>Francisco Bilbao 255</t>
         </is>
       </c>
       <c r="G16" s="14" t="inlineStr">
@@ -1182,11 +1175,11 @@
         </is>
       </c>
       <c r="H16" s="14" t="n">
-        <v>972078066</v>
+        <v>990847901</v>
       </c>
       <c r="I16" s="14" t="inlineStr">
         <is>
-          <t>10 a 19</t>
+          <t>9 a 13 y de 14 a 17</t>
         </is>
       </c>
       <c r="J16" s="16" t="n"/>
@@ -1196,37 +1189,37 @@
         <v>20250318</v>
       </c>
       <c r="B17" s="15" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D17" s="15" t="inlineStr">
         <is>
-          <t>77.141.688-8</t>
+          <t>78.074.427-8</t>
         </is>
       </c>
       <c r="E17" s="15" t="inlineStr">
         <is>
-          <t>Servicios Sociales Sur Spa</t>
+          <t>serv. Odontologicos Loreto sanz</t>
         </is>
       </c>
       <c r="F17" s="15" t="inlineStr">
         <is>
-          <t>Francisco Bilbao 255</t>
+          <t>Santa rosa 575 of 27</t>
         </is>
       </c>
       <c r="G17" s="14" t="inlineStr">
         <is>
-          <t>Puerto Montt</t>
+          <t>Puerto Varas</t>
         </is>
       </c>
       <c r="H17" s="14" t="n">
-        <v>990847901</v>
+        <v>982188029</v>
       </c>
       <c r="I17" s="14" t="inlineStr">
         <is>
-          <t>9 a 13 y de 14 a 17</t>
+          <t>10 a 18</t>
         </is>
       </c>
       <c r="J17" s="16" t="n"/>
@@ -1238,50 +1231,94 @@
       <c r="B18" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="C18" s="15" t="n">
-        <v>60</v>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>78.074.427-8</t>
+          <t>17.673.326-8</t>
         </is>
       </c>
       <c r="E18" s="15" t="inlineStr">
         <is>
-          <t>serv. Odontologicos Loreto sanz</t>
+          <t>Maria José Rodriguez</t>
         </is>
       </c>
       <c r="F18" s="15" t="inlineStr">
         <is>
-          <t>Santa rosa 575 of 27</t>
+          <t>Colaco s/n km 3, parcela 9</t>
         </is>
       </c>
       <c r="G18" s="14" t="inlineStr">
         <is>
-          <t>Puerto Varas</t>
-        </is>
-      </c>
-      <c r="H18" s="14" t="n">
-        <v>982188029</v>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="H18" s="14" t="inlineStr">
+        <is>
+          <t>972861950</t>
+        </is>
       </c>
       <c r="I18" s="14" t="inlineStr">
         <is>
-          <t>10 a 18</t>
-        </is>
-      </c>
-      <c r="J18" s="16" t="n"/>
+          <t>Cliente test</t>
+        </is>
+      </c>
+      <c r="J18" s="16" t="inlineStr">
+        <is>
+          <t>1002</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="11">
-      <c r="A19" s="14" t="n"/>
-      <c r="B19" s="15" t="n"/>
-      <c r="C19" s="15" t="n"/>
-      <c r="D19" s="15" t="n"/>
-      <c r="E19" s="15" t="n"/>
-      <c r="F19" s="15" t="n"/>
-      <c r="G19" s="14" t="n"/>
-      <c r="H19" s="14" t="n"/>
-      <c r="I19" s="14" t="n"/>
-      <c r="J19" s="16" t="n"/>
+      <c r="A19" s="14" t="n">
+        <v>20250318</v>
+      </c>
+      <c r="B19" s="15" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" s="15" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D19" s="15" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="E19" s="15" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="F19" s="15" t="inlineStr">
+        <is>
+          <t>Colaco s/n km 3, parcela 9</t>
+        </is>
+      </c>
+      <c r="G19" s="14" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="H19" s="14" t="inlineStr">
+        <is>
+          <t>988809704</t>
+        </is>
+      </c>
+      <c r="I19" s="14" t="inlineStr">
+        <is>
+          <t>Cliente test</t>
+        </is>
+      </c>
+      <c r="J19" s="16" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="11">
       <c r="A20" s="14" t="n"/>
@@ -1812,16 +1849,16 @@
       <c r="J63" s="16" t="n"/>
     </row>
     <row r="64" ht="15.75" customHeight="1" s="11">
-      <c r="A64" s="14" t="n"/>
+      <c r="A64" s="15" t="n"/>
       <c r="B64" s="15" t="n"/>
       <c r="C64" s="15" t="n"/>
       <c r="D64" s="15" t="n"/>
       <c r="E64" s="15" t="n"/>
       <c r="F64" s="15" t="n"/>
-      <c r="G64" s="14" t="n"/>
-      <c r="H64" s="14" t="n"/>
-      <c r="I64" s="14" t="n"/>
-      <c r="J64" s="16" t="n"/>
+      <c r="G64" s="15" t="n"/>
+      <c r="H64" s="15" t="n"/>
+      <c r="I64" s="15" t="n"/>
+      <c r="J64" s="15" t="n"/>
     </row>
     <row r="65" ht="15.75" customHeight="1" s="11">
       <c r="A65" s="15" t="n"/>
@@ -2699,18 +2736,7 @@
       <c r="I137" s="15" t="n"/>
       <c r="J137" s="15" t="n"/>
     </row>
-    <row r="138" ht="15" customHeight="1" s="11">
-      <c r="A138" s="15" t="n"/>
-      <c r="B138" s="15" t="n"/>
-      <c r="C138" s="15" t="n"/>
-      <c r="D138" s="15" t="n"/>
-      <c r="E138" s="15" t="n"/>
-      <c r="F138" s="15" t="n"/>
-      <c r="G138" s="15" t="n"/>
-      <c r="H138" s="15" t="n"/>
-      <c r="I138" s="15" t="n"/>
-      <c r="J138" s="15" t="n"/>
-    </row>
+    <row r="138" ht="15" customHeight="1" s="11"/>
     <row r="139" ht="15" customHeight="1" s="11"/>
     <row r="140" ht="15" customHeight="1" s="11"/>
     <row r="141" ht="15" customHeight="1" s="11"/>

</xml_diff>

<commit_message>
Agregando app con modificaciones
Se agregan funcionalidades de segregacion
de funciones por privilegios. Se agrega
cuenta invitado
</commit_message>
<xml_diff>
--- a/bd/ruta.xlsx
+++ b/bd/ruta.xlsx
@@ -514,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L138"/>
+  <dimension ref="A1:L137"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -613,125 +613,116 @@
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="11">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>20250318</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D3" s="9" t="inlineStr">
         <is>
           <t>9999</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ACHS Osorno</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Av Zenteno 1529</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Osorno</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>DOCTOR SIMI</t>
+        </is>
+      </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>mall valdivia</t>
+        </is>
+      </c>
+      <c r="G3" s="9" t="inlineStr">
+        <is>
+          <t>valdivia</t>
+        </is>
+      </c>
+      <c r="H3" s="9" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="9" t="inlineStr">
+        <is>
+          <t>SERVICIO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="J3" s="9" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="11">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>20250318</t>
-        </is>
-      </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t>9999</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>DOCTOR SIMI</t>
-        </is>
-      </c>
-      <c r="F4" s="9" t="inlineStr">
-        <is>
-          <t>mall valdivia</t>
-        </is>
-      </c>
-      <c r="G4" s="9" t="inlineStr">
-        <is>
-          <t>valdivia</t>
-        </is>
-      </c>
-      <c r="H4" s="9" t="inlineStr">
+      <c r="A4" s="14" t="n">
+        <v>20250318</v>
+      </c>
+      <c r="B4" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15" t="n">
+        <v>9999</v>
+      </c>
+      <c r="E4" s="15" t="inlineStr">
+        <is>
+          <t>ACHS VALDIVIA</t>
+        </is>
+      </c>
+      <c r="F4" s="15" t="inlineStr">
+        <is>
+          <t>Beauchef Nº705, Valdivia</t>
+        </is>
+      </c>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t>Valdivia</t>
+        </is>
+      </c>
+      <c r="H4" s="14" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I4" s="9" t="inlineStr">
-        <is>
-          <t>SERVICIO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="J4" s="9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="I4" s="14" t="n"/>
+      <c r="J4" s="16" t="n"/>
     </row>
     <row r="5" ht="15" customHeight="1" s="11">
       <c r="A5" s="14" t="n">
         <v>20250318</v>
       </c>
       <c r="B5" s="15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>15</v>
-      </c>
-      <c r="D5" s="15" t="n">
-        <v>9999</v>
+        <v>60</v>
+      </c>
+      <c r="D5" s="15" t="inlineStr">
+        <is>
+          <t>77.880.747-5</t>
+        </is>
       </c>
       <c r="E5" s="15" t="inlineStr">
         <is>
-          <t>ACHS VALDIVIA</t>
+          <t>Salud Humana Pablo Contreras</t>
         </is>
       </c>
       <c r="F5" s="15" t="inlineStr">
         <is>
-          <t>Beauchef Nº705, Valdivia</t>
+          <t>beauchef 925  ( nueva direccion)</t>
         </is>
       </c>
       <c r="G5" s="14" t="inlineStr">
@@ -739,12 +730,14 @@
           <t>Valdivia</t>
         </is>
       </c>
-      <c r="H5" s="14" t="inlineStr">
+      <c r="H5" s="14" t="n">
+        <v>966796589</v>
+      </c>
+      <c r="I5" s="14" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I5" s="14" t="n"/>
       <c r="J5" s="16" t="n"/>
     </row>
     <row r="6" ht="15" customHeight="1" s="11">
@@ -752,24 +745,24 @@
         <v>20250318</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D6" s="15" t="inlineStr">
         <is>
-          <t>77.880.747-5</t>
+          <t>77.624.403-1</t>
         </is>
       </c>
       <c r="E6" s="15" t="inlineStr">
         <is>
-          <t>Salud Humana Pablo Contreras</t>
+          <t>serv para salud humana Gloria Jofré EIRL</t>
         </is>
       </c>
       <c r="F6" s="15" t="inlineStr">
         <is>
-          <t>beauchef 925  ( nueva direccion)</t>
+          <t>García Reyes 686</t>
         </is>
       </c>
       <c r="G6" s="14" t="inlineStr">
@@ -778,11 +771,11 @@
         </is>
       </c>
       <c r="H6" s="14" t="n">
-        <v>966796589</v>
+        <v>952541245</v>
       </c>
       <c r="I6" s="14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>DEUDA</t>
         </is>
       </c>
       <c r="J6" s="16" t="n"/>
@@ -792,37 +785,37 @@
         <v>20250318</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D7" s="15" t="inlineStr">
         <is>
-          <t>77.624.403-1</t>
+          <t>65.062.843-8</t>
         </is>
       </c>
       <c r="E7" s="15" t="inlineStr">
         <is>
-          <t>serv para salud humana Gloria Jofré EIRL</t>
+          <t>Fundacion salud y Familia</t>
         </is>
       </c>
       <c r="F7" s="15" t="inlineStr">
         <is>
-          <t>García Reyes 686</t>
+          <t>Benavente 379 of 206</t>
         </is>
       </c>
       <c r="G7" s="14" t="inlineStr">
         <is>
-          <t>Valdivia</t>
+          <t>Puerto Montt</t>
         </is>
       </c>
       <c r="H7" s="14" t="n">
-        <v>952541245</v>
+        <v>987516103</v>
       </c>
       <c r="I7" s="14" t="inlineStr">
         <is>
-          <t>DEUDA</t>
+          <t>a las 16:00 / nesecita 100 bolsas amarillas</t>
         </is>
       </c>
       <c r="J7" s="16" t="n"/>
@@ -832,24 +825,22 @@
         <v>20250318</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="15" t="inlineStr">
-        <is>
-          <t>65.062.843-8</t>
-        </is>
+        <v>15</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>9999</v>
       </c>
       <c r="E8" s="15" t="inlineStr">
         <is>
-          <t>Fundacion salud y Familia</t>
+          <t>ACHS PUERTO MONTT</t>
         </is>
       </c>
       <c r="F8" s="15" t="inlineStr">
         <is>
-          <t>Benavente 379 of 206</t>
+          <t>Ejército Nº360</t>
         </is>
       </c>
       <c r="G8" s="14" t="inlineStr">
@@ -857,14 +848,12 @@
           <t>Puerto Montt</t>
         </is>
       </c>
-      <c r="H8" s="14" t="n">
-        <v>987516103</v>
-      </c>
-      <c r="I8" s="14" t="inlineStr">
-        <is>
-          <t>a las 16:00 / nesecita 100 bolsas amarillas</t>
-        </is>
-      </c>
+      <c r="H8" s="14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" s="14" t="n"/>
       <c r="J8" s="16" t="n"/>
     </row>
     <row r="9" ht="15" customHeight="1" s="11">
@@ -872,22 +861,22 @@
         <v>20250318</v>
       </c>
       <c r="B9" s="15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="15" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>9999</v>
       </c>
       <c r="E9" s="15" t="inlineStr">
         <is>
-          <t>ACHS PUERTO MONTT</t>
+          <t>EVEREST PTO MONTT</t>
         </is>
       </c>
       <c r="F9" s="15" t="inlineStr">
         <is>
-          <t>Ejército Nº360</t>
+          <t>Juan Soler Manfredini L 131</t>
         </is>
       </c>
       <c r="G9" s="14" t="inlineStr">
@@ -900,7 +889,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I9" s="14" t="n"/>
+      <c r="I9" s="14" t="inlineStr">
+        <is>
+          <t>8:30 a 13 y 14 a 19</t>
+        </is>
+      </c>
       <c r="J9" s="16" t="n"/>
     </row>
     <row r="10" ht="15" customHeight="1" s="11">
@@ -908,22 +901,24 @@
         <v>20250318</v>
       </c>
       <c r="B10" s="15" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="15" t="n">
         <v>30</v>
       </c>
-      <c r="D10" s="15" t="n">
-        <v>9999</v>
+      <c r="D10" s="15" t="inlineStr">
+        <is>
+          <t>65.062.843-8</t>
+        </is>
       </c>
       <c r="E10" s="15" t="inlineStr">
         <is>
-          <t>EVEREST PTO MONTT</t>
+          <t>CESFAM San Pablo</t>
         </is>
       </c>
       <c r="F10" s="15" t="inlineStr">
         <is>
-          <t>Juan Soler Manfredini L 131</t>
+          <t>Barrancas S/N mirasol</t>
         </is>
       </c>
       <c r="G10" s="14" t="inlineStr">
@@ -931,14 +926,12 @@
           <t>Puerto Montt</t>
         </is>
       </c>
-      <c r="H10" s="14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="H10" s="14" t="n">
+        <v>990579442</v>
       </c>
       <c r="I10" s="14" t="inlineStr">
         <is>
-          <t>8:30 a 13 y 14 a 19</t>
+          <t>9:30 a 14 y 17:30 a 20</t>
         </is>
       </c>
       <c r="J10" s="16" t="n"/>
@@ -948,24 +941,24 @@
         <v>20250318</v>
       </c>
       <c r="B11" s="15" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="15" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>65.062.843-8</t>
+          <t>77.628.398-3</t>
         </is>
       </c>
       <c r="E11" s="15" t="inlineStr">
         <is>
-          <t>CESFAM San Pablo</t>
+          <t>CLINICA ODONTOLOGICA ACDENT SPA</t>
         </is>
       </c>
       <c r="F11" s="15" t="inlineStr">
         <is>
-          <t>Barrancas S/N mirasol</t>
+          <t>Antonio Varas 55 of 509</t>
         </is>
       </c>
       <c r="G11" s="14" t="inlineStr">
@@ -973,12 +966,14 @@
           <t>Puerto Montt</t>
         </is>
       </c>
-      <c r="H11" s="14" t="n">
-        <v>990579442</v>
+      <c r="H11" s="14" t="inlineStr">
+        <is>
+          <t>964988313/967120480</t>
+        </is>
       </c>
       <c r="I11" s="14" t="inlineStr">
         <is>
-          <t>9:30 a 14 y 17:30 a 20</t>
+          <t>10 a 13 y 15 a 17:30</t>
         </is>
       </c>
       <c r="J11" s="16" t="n"/>
@@ -988,24 +983,24 @@
         <v>20250318</v>
       </c>
       <c r="B12" s="15" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>77.628.398-3</t>
+          <t>77.491.661-k</t>
         </is>
       </c>
       <c r="E12" s="15" t="inlineStr">
         <is>
-          <t>CLINICA ODONTOLOGICA ACDENT SPA</t>
+          <t>Emuna soluciones medicas spa</t>
         </is>
       </c>
       <c r="F12" s="15" t="inlineStr">
         <is>
-          <t>Antonio Varas 55 of 509</t>
+          <t>Benavente 840,Of 605</t>
         </is>
       </c>
       <c r="G12" s="14" t="inlineStr">
@@ -1015,12 +1010,12 @@
       </c>
       <c r="H12" s="14" t="inlineStr">
         <is>
-          <t>964988313/967120480</t>
+          <t>962826997/951701572</t>
         </is>
       </c>
       <c r="I12" s="14" t="inlineStr">
         <is>
-          <t>10 a 13 y 15 a 17:30</t>
+          <t>9 a 13 y 14 a 16:00</t>
         </is>
       </c>
       <c r="J12" s="16" t="n"/>
@@ -1030,24 +1025,24 @@
         <v>20250318</v>
       </c>
       <c r="B13" s="15" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D13" s="15" t="inlineStr">
         <is>
-          <t>77.491.661-k</t>
+          <t>76.058.615-3</t>
         </is>
       </c>
       <c r="E13" s="15" t="inlineStr">
         <is>
-          <t>Emuna soluciones medicas spa</t>
+          <t>Fernandez y Haussmann odontologia</t>
         </is>
       </c>
       <c r="F13" s="15" t="inlineStr">
         <is>
-          <t>Benavente 840,Of 605</t>
+          <t>Quillota 175 of 1110</t>
         </is>
       </c>
       <c r="G13" s="14" t="inlineStr">
@@ -1057,12 +1052,12 @@
       </c>
       <c r="H13" s="14" t="inlineStr">
         <is>
-          <t>962826997/951701572</t>
+          <t>652263740/934533835</t>
         </is>
       </c>
       <c r="I13" s="14" t="inlineStr">
         <is>
-          <t>9 a 13 y 14 a 16:00</t>
+          <t>10 a 18</t>
         </is>
       </c>
       <c r="J13" s="16" t="n"/>
@@ -1072,24 +1067,24 @@
         <v>20250318</v>
       </c>
       <c r="B14" s="15" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D14" s="15" t="inlineStr">
         <is>
-          <t>76.058.615-3</t>
+          <t>78.034.130-0</t>
         </is>
       </c>
       <c r="E14" s="15" t="inlineStr">
         <is>
-          <t>Fernandez y Haussmann odontologia</t>
+          <t>KARUS</t>
         </is>
       </c>
       <c r="F14" s="15" t="inlineStr">
         <is>
-          <t>Quillota 175 of 1110</t>
+          <t>Juan soler manfredini 41 of 1803</t>
         </is>
       </c>
       <c r="G14" s="14" t="inlineStr">
@@ -1099,12 +1094,12 @@
       </c>
       <c r="H14" s="14" t="inlineStr">
         <is>
-          <t>652263740/934533835</t>
+          <t>952296251/957121954</t>
         </is>
       </c>
       <c r="I14" s="14" t="inlineStr">
         <is>
-          <t>10 a 18</t>
+          <t>cliente nuevo 1C Y 1B /11 a  14</t>
         </is>
       </c>
       <c r="J14" s="16" t="n"/>
@@ -1114,24 +1109,24 @@
         <v>20250318</v>
       </c>
       <c r="B15" s="15" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D15" s="15" t="inlineStr">
         <is>
-          <t>78.034.130-0</t>
+          <t>77.962.205-3</t>
         </is>
       </c>
       <c r="E15" s="15" t="inlineStr">
         <is>
-          <t>KARUS</t>
+          <t>we face and body spa.</t>
         </is>
       </c>
       <c r="F15" s="15" t="inlineStr">
         <is>
-          <t>Juan soler manfredini 41 of 1803</t>
+          <t>O´higgins 167 of 609</t>
         </is>
       </c>
       <c r="G15" s="14" t="inlineStr">
@@ -1139,14 +1134,12 @@
           <t>Puerto Montt</t>
         </is>
       </c>
-      <c r="H15" s="14" t="inlineStr">
-        <is>
-          <t>952296251/957121954</t>
-        </is>
+      <c r="H15" s="14" t="n">
+        <v>972078066</v>
       </c>
       <c r="I15" s="14" t="inlineStr">
         <is>
-          <t>cliente nuevo 1C Y 1B /11 a  14</t>
+          <t>10 a 19</t>
         </is>
       </c>
       <c r="J15" s="16" t="n"/>
@@ -1156,24 +1149,24 @@
         <v>20250318</v>
       </c>
       <c r="B16" s="15" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D16" s="15" t="inlineStr">
         <is>
-          <t>77.962.205-3</t>
+          <t>77.141.688-8</t>
         </is>
       </c>
       <c r="E16" s="15" t="inlineStr">
         <is>
-          <t>we face and body spa.</t>
+          <t>Servicios Sociales Sur Spa</t>
         </is>
       </c>
       <c r="F16" s="15" t="inlineStr">
         <is>
-          <t>O´higgins 167 of 609</t>
+          <t>Francisco Bilbao 255</t>
         </is>
       </c>
       <c r="G16" s="14" t="inlineStr">
@@ -1182,11 +1175,11 @@
         </is>
       </c>
       <c r="H16" s="14" t="n">
-        <v>972078066</v>
+        <v>990847901</v>
       </c>
       <c r="I16" s="14" t="inlineStr">
         <is>
-          <t>10 a 19</t>
+          <t>9 a 13 y de 14 a 17</t>
         </is>
       </c>
       <c r="J16" s="16" t="n"/>
@@ -1196,37 +1189,37 @@
         <v>20250318</v>
       </c>
       <c r="B17" s="15" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="15" t="n">
         <v>60</v>
       </c>
       <c r="D17" s="15" t="inlineStr">
         <is>
-          <t>77.141.688-8</t>
+          <t>78.074.427-8</t>
         </is>
       </c>
       <c r="E17" s="15" t="inlineStr">
         <is>
-          <t>Servicios Sociales Sur Spa</t>
+          <t>serv. Odontologicos Loreto sanz</t>
         </is>
       </c>
       <c r="F17" s="15" t="inlineStr">
         <is>
-          <t>Francisco Bilbao 255</t>
+          <t>Santa rosa 575 of 27</t>
         </is>
       </c>
       <c r="G17" s="14" t="inlineStr">
         <is>
-          <t>Puerto Montt</t>
+          <t>Puerto Varas</t>
         </is>
       </c>
       <c r="H17" s="14" t="n">
-        <v>990847901</v>
+        <v>982188029</v>
       </c>
       <c r="I17" s="14" t="inlineStr">
         <is>
-          <t>9 a 13 y de 14 a 17</t>
+          <t>10 a 18</t>
         </is>
       </c>
       <c r="J17" s="16" t="n"/>
@@ -1238,50 +1231,94 @@
       <c r="B18" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="C18" s="15" t="n">
-        <v>60</v>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>78.074.427-8</t>
+          <t>17.673.326-8</t>
         </is>
       </c>
       <c r="E18" s="15" t="inlineStr">
         <is>
-          <t>serv. Odontologicos Loreto sanz</t>
+          <t>Maria José Rodriguez</t>
         </is>
       </c>
       <c r="F18" s="15" t="inlineStr">
         <is>
-          <t>Santa rosa 575 of 27</t>
+          <t>Colaco s/n km 3, parcela 9</t>
         </is>
       </c>
       <c r="G18" s="14" t="inlineStr">
         <is>
-          <t>Puerto Varas</t>
-        </is>
-      </c>
-      <c r="H18" s="14" t="n">
-        <v>982188029</v>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="H18" s="14" t="inlineStr">
+        <is>
+          <t>972861950</t>
+        </is>
       </c>
       <c r="I18" s="14" t="inlineStr">
         <is>
-          <t>10 a 18</t>
-        </is>
-      </c>
-      <c r="J18" s="16" t="n"/>
+          <t>Cliente test</t>
+        </is>
+      </c>
+      <c r="J18" s="16" t="inlineStr">
+        <is>
+          <t>1002</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="11">
-      <c r="A19" s="14" t="n"/>
-      <c r="B19" s="15" t="n"/>
-      <c r="C19" s="15" t="n"/>
-      <c r="D19" s="15" t="n"/>
-      <c r="E19" s="15" t="n"/>
-      <c r="F19" s="15" t="n"/>
-      <c r="G19" s="14" t="n"/>
-      <c r="H19" s="14" t="n"/>
-      <c r="I19" s="14" t="n"/>
-      <c r="J19" s="16" t="n"/>
+      <c r="A19" s="14" t="n">
+        <v>20250318</v>
+      </c>
+      <c r="B19" s="15" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" s="15" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D19" s="15" t="inlineStr">
+        <is>
+          <t>16.742.249-7</t>
+        </is>
+      </c>
+      <c r="E19" s="15" t="inlineStr">
+        <is>
+          <t>Isaias Beroiza Mora</t>
+        </is>
+      </c>
+      <c r="F19" s="15" t="inlineStr">
+        <is>
+          <t>Colaco s/n km 3, parcela 9</t>
+        </is>
+      </c>
+      <c r="G19" s="14" t="inlineStr">
+        <is>
+          <t>Calbuco</t>
+        </is>
+      </c>
+      <c r="H19" s="14" t="inlineStr">
+        <is>
+          <t>988809704</t>
+        </is>
+      </c>
+      <c r="I19" s="14" t="inlineStr">
+        <is>
+          <t>Cliente test</t>
+        </is>
+      </c>
+      <c r="J19" s="16" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="11">
       <c r="A20" s="14" t="n"/>
@@ -1812,16 +1849,16 @@
       <c r="J63" s="16" t="n"/>
     </row>
     <row r="64" ht="15.75" customHeight="1" s="11">
-      <c r="A64" s="14" t="n"/>
+      <c r="A64" s="15" t="n"/>
       <c r="B64" s="15" t="n"/>
       <c r="C64" s="15" t="n"/>
       <c r="D64" s="15" t="n"/>
       <c r="E64" s="15" t="n"/>
       <c r="F64" s="15" t="n"/>
-      <c r="G64" s="14" t="n"/>
-      <c r="H64" s="14" t="n"/>
-      <c r="I64" s="14" t="n"/>
-      <c r="J64" s="16" t="n"/>
+      <c r="G64" s="15" t="n"/>
+      <c r="H64" s="15" t="n"/>
+      <c r="I64" s="15" t="n"/>
+      <c r="J64" s="15" t="n"/>
     </row>
     <row r="65" ht="15.75" customHeight="1" s="11">
       <c r="A65" s="15" t="n"/>
@@ -2699,18 +2736,7 @@
       <c r="I137" s="15" t="n"/>
       <c r="J137" s="15" t="n"/>
     </row>
-    <row r="138" ht="15" customHeight="1" s="11">
-      <c r="A138" s="15" t="n"/>
-      <c r="B138" s="15" t="n"/>
-      <c r="C138" s="15" t="n"/>
-      <c r="D138" s="15" t="n"/>
-      <c r="E138" s="15" t="n"/>
-      <c r="F138" s="15" t="n"/>
-      <c r="G138" s="15" t="n"/>
-      <c r="H138" s="15" t="n"/>
-      <c r="I138" s="15" t="n"/>
-      <c r="J138" s="15" t="n"/>
-    </row>
+    <row r="138" ht="15" customHeight="1" s="11"/>
     <row r="139" ht="15" customHeight="1" s="11"/>
     <row r="140" ht="15" customHeight="1" s="11"/>
     <row r="141" ht="15" customHeight="1" s="11"/>

</xml_diff>